<commit_message>
Adding ground truth test set values
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_test_set.xlsx
+++ b/GHT/ground_truth_detection_pts_test_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7CF863-0826-4BE4-AB7C-375C642A9F46}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17202E26-A59C-48B8-9FBC-9B5C1DF9EC0B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -464,198 +464,198 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>6067977</v>
+        <v>6186286</v>
       </c>
       <c r="B3" s="2">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>6095054</v>
+        <v>6242975</v>
       </c>
       <c r="B4" s="2">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>6173842</v>
+        <v>6254655</v>
       </c>
       <c r="B5" s="2">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>6201211</v>
+        <v>6293323</v>
       </c>
       <c r="B6" s="2">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>6218246</v>
+        <v>6358896</v>
       </c>
       <c r="B7" s="2">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>6268647</v>
+        <v>6393163</v>
       </c>
       <c r="B8" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>6490491</v>
+        <v>6717781</v>
       </c>
       <c r="B9" s="2">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>6729799</v>
+        <v>9189512</v>
       </c>
       <c r="B10" s="2">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>6828936</v>
+        <v>9185492</v>
       </c>
       <c r="B11" s="2">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>6868398</v>
+        <v>9157873</v>
       </c>
       <c r="B12" s="2">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>6881614</v>
+        <v>9156077</v>
       </c>
       <c r="B13" s="2">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2">
         <v>56</v>
       </c>
       <c r="D13" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>6993961</v>
+        <v>9155692</v>
       </c>
       <c r="B14" s="2">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>7081341</v>
+        <v>9118221</v>
       </c>
       <c r="B15" s="2">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>7222303</v>
+        <v>9109922</v>
       </c>
       <c r="B16" s="2">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="D16" s="2">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -663,13 +663,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>7257259</v>
+        <v>9096172</v>
       </c>
       <c r="B17" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2">
         <v>24</v>
@@ -677,213 +677,129 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>7299268</v>
+        <v>9073089</v>
       </c>
       <c r="B18" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D18" s="2">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>7316415</v>
+        <v>9073037</v>
       </c>
       <c r="B19" s="2">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C19" s="2">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>7337296</v>
+        <v>9065075</v>
       </c>
       <c r="B20" s="2">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C20" s="2">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>7396455</v>
+        <v>9064027</v>
       </c>
       <c r="B21" s="2">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>7444276</v>
+        <v>9058432</v>
       </c>
       <c r="B22" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D22" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
-        <v>7466141</v>
-      </c>
-      <c r="B23" s="2">
-        <v>27</v>
-      </c>
-      <c r="C23" s="2">
-        <v>63</v>
-      </c>
-      <c r="D23" s="2">
-        <v>22</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
-        <v>7489680</v>
-      </c>
-      <c r="B24" s="2">
-        <v>31</v>
-      </c>
-      <c r="C24" s="2">
-        <v>55</v>
-      </c>
-      <c r="D24" s="2">
-        <v>19</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
-        <v>7496249</v>
-      </c>
-      <c r="B25" s="2">
-        <v>21</v>
-      </c>
-      <c r="C25" s="2">
-        <v>51</v>
-      </c>
-      <c r="D25" s="2">
-        <v>21</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
-        <v>7499820</v>
-      </c>
-      <c r="B26" s="2">
-        <v>31</v>
-      </c>
-      <c r="C26" s="2">
-        <v>50</v>
-      </c>
-      <c r="D26" s="2">
-        <v>21</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
-        <v>7629097</v>
-      </c>
-      <c r="B27" s="2">
-        <v>31</v>
-      </c>
-      <c r="C27" s="2">
-        <v>42</v>
-      </c>
-      <c r="D27" s="2">
-        <v>15</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
-        <v>7796800</v>
-      </c>
-      <c r="B28" s="2">
-        <v>27</v>
-      </c>
-      <c r="C28" s="2">
-        <v>53</v>
-      </c>
-      <c r="D28" s="2">
-        <v>17</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
-        <v>7800424</v>
-      </c>
-      <c r="B29" s="2">
-        <v>17</v>
-      </c>
-      <c r="C29">
-        <v>50</v>
-      </c>
-      <c r="D29" s="2">
-        <v>21</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
-        <v>7887075</v>
-      </c>
-      <c r="B30" s="2">
-        <v>36</v>
-      </c>
-      <c r="C30">
-        <v>60</v>
-      </c>
-      <c r="D30" s="2">
-        <v>20</v>
-      </c>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
-        <v>7958084</v>
-      </c>
-      <c r="B31" s="2">
-        <v>32</v>
-      </c>
-      <c r="C31">
-        <v>54</v>
-      </c>
-      <c r="D31" s="2">
-        <v>17</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
-        <v>7962433</v>
-      </c>
-      <c r="B32" s="2">
-        <v>29</v>
-      </c>
-      <c r="C32">
-        <v>63</v>
-      </c>
-      <c r="D32" s="2">
-        <v>20</v>
-      </c>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>

</xml_diff>

<commit_message>
Making 40 validation set
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts_test_set.xlsx
+++ b/GHT/ground_truth_detection_pts_test_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17202E26-A59C-48B8-9FBC-9B5C1DF9EC0B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626148DB-C7AB-4560-A2D2-8AA4826AFA16}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -746,107 +746,290 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="A23" s="2">
+        <v>9056633</v>
+      </c>
+      <c r="B23" s="2">
+        <v>30</v>
+      </c>
+      <c r="C23" s="2">
+        <v>57</v>
+      </c>
+      <c r="D23" s="2">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="2">
+        <v>9038021</v>
+      </c>
+      <c r="B24" s="2">
+        <v>25</v>
+      </c>
+      <c r="C24" s="2">
+        <v>31</v>
+      </c>
+      <c r="D24" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="A25" s="2">
+        <v>9028403</v>
+      </c>
+      <c r="B25" s="2">
+        <v>21</v>
+      </c>
+      <c r="C25" s="2">
+        <v>42</v>
+      </c>
+      <c r="D25" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="A26" s="2">
+        <v>8977015</v>
+      </c>
+      <c r="B26" s="2">
+        <v>31</v>
+      </c>
+      <c r="C26" s="2">
+        <v>57</v>
+      </c>
+      <c r="D26" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="A27" s="2">
+        <v>8968387</v>
+      </c>
+      <c r="B27" s="2">
+        <v>32</v>
+      </c>
+      <c r="C27" s="2">
+        <v>54</v>
+      </c>
+      <c r="D27" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="A28" s="2">
+        <v>8920704</v>
+      </c>
+      <c r="B28" s="2">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2">
+        <v>54</v>
+      </c>
+      <c r="D28" s="2">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="A29" s="2">
+        <v>8920679</v>
+      </c>
+      <c r="B29" s="2">
+        <v>26</v>
+      </c>
+      <c r="C29" s="2">
+        <v>54</v>
+      </c>
+      <c r="D29" s="2">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="A30" s="2">
+        <v>8840552</v>
+      </c>
+      <c r="B30" s="2">
+        <v>24</v>
+      </c>
+      <c r="C30" s="2">
+        <v>46</v>
+      </c>
+      <c r="D30" s="2">
+        <v>21</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="A31" s="2">
+        <v>8781623</v>
+      </c>
+      <c r="B31" s="2">
+        <v>29</v>
+      </c>
+      <c r="C31" s="2">
+        <v>35</v>
+      </c>
+      <c r="D31" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>8765787</v>
+      </c>
+      <c r="B32" s="2">
+        <v>29</v>
+      </c>
+      <c r="C32" s="2">
+        <v>46</v>
+      </c>
+      <c r="D32" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>8602870</v>
+      </c>
+      <c r="B33" s="2">
+        <v>38</v>
+      </c>
+      <c r="C33" s="2">
+        <v>48</v>
+      </c>
+      <c r="D33" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>8602775</v>
+      </c>
+      <c r="B34" s="2">
+        <v>24</v>
+      </c>
+      <c r="C34" s="2">
+        <v>47</v>
+      </c>
+      <c r="D34" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>8709670</v>
+      </c>
+      <c r="B35" s="2">
+        <v>28</v>
+      </c>
+      <c r="C35" s="2">
+        <v>64</v>
+      </c>
+      <c r="D35" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>8699113</v>
+      </c>
+      <c r="B36" s="2">
+        <v>32</v>
+      </c>
+      <c r="C36" s="2">
+        <v>46</v>
+      </c>
+      <c r="D36" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>8666330</v>
+      </c>
+      <c r="B37" s="2">
+        <v>26</v>
+      </c>
+      <c r="C37" s="2">
+        <v>45</v>
+      </c>
+      <c r="D37" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>8665805</v>
+      </c>
+      <c r="B38" s="2">
+        <v>31</v>
+      </c>
+      <c r="C38" s="2">
+        <v>47</v>
+      </c>
+      <c r="D38" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>8665616</v>
+      </c>
+      <c r="B39" s="2">
+        <v>29</v>
+      </c>
+      <c r="C39" s="2">
+        <v>38</v>
+      </c>
+      <c r="D39" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>8662841</v>
+      </c>
+      <c r="B40" s="2">
+        <v>27</v>
+      </c>
+      <c r="C40" s="2">
+        <v>48</v>
+      </c>
+      <c r="D40" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>8636498</v>
+      </c>
+      <c r="B41" s="2">
+        <v>36</v>
+      </c>
+      <c r="C41" s="2">
+        <v>46</v>
+      </c>
+      <c r="D41" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>